<commit_message>
WIP: add additional tests
</commit_message>
<xml_diff>
--- a/tests/input/bootstrap26.xlsx
+++ b/tests/input/bootstrap26.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="390" windowWidth="15855" windowHeight="8895"/>
+    <workbookView xWindow="240" yWindow="135" windowWidth="16095" windowHeight="9150"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -357,13 +357,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="C3"/>
+  <dimension ref="C3:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="9.140625" style="1"/>
+    <col min="3" max="4" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="3:3">

</xml_diff>